<commit_message>
commiting all files related to wor entity - vandana task  as well as all other files
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Client Admin Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Client Admin Suite.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="555">
   <si>
     <t>TCID</t>
   </si>
@@ -2316,7 +2316,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2357,9 @@
       <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -2381,7 +2383,9 @@
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -2393,7 +2397,9 @@
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -2406,7 +2412,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2420,7 +2426,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2434,7 +2440,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2448,7 +2454,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2462,7 +2468,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2643,7 +2649,9 @@
       <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -2655,7 +2663,9 @@
       <c r="C26" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
@@ -2667,7 +2677,9 @@
       <c r="C27" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -2679,7 +2691,9 @@
       <c r="C28" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
@@ -2691,7 +2705,9 @@
       <c r="C29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -2703,7 +2719,9 @@
       <c r="C30" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="9"/>
+      <c r="D30" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
@@ -2715,7 +2733,9 @@
       <c r="C31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="9"/>
+      <c r="D31" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -2727,7 +2747,9 @@
       <c r="C32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="9"/>
+      <c r="D32" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -2739,7 +2761,9 @@
       <c r="C33" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="9"/>
+      <c r="D33" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
@@ -2751,7 +2775,9 @@
       <c r="C34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="9"/>
+      <c r="D34" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
@@ -2763,7 +2789,9 @@
       <c r="C35" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="9"/>
+      <c r="D35" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
@@ -2775,7 +2803,9 @@
       <c r="C36" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="9"/>
+      <c r="D36" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
@@ -2787,7 +2817,9 @@
       <c r="C37" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="9"/>
+      <c r="D37" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
@@ -2799,7 +2831,9 @@
       <c r="C38" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="9"/>
+      <c r="D38" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
@@ -2811,7 +2845,9 @@
       <c r="C39" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="9"/>
+      <c r="D39" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
@@ -2823,7 +2859,9 @@
       <c r="C40" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
@@ -3651,7 +3689,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="D3" s="4"/>
     </row>
@@ -3856,7 +3894,7 @@
         <v>3</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="W3" s="4"/>
     </row>
@@ -3881,7 +3919,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="25.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -3913,7 +3951,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3929,7 +3969,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3945,7 +3987,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3961,7 +4005,9 @@
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F5" s="4"/>
     </row>
   </sheetData>
@@ -4085,7 +4131,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -4117,7 +4163,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4133,7 +4181,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4149,7 +4199,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -4256,7 +4308,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="35.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -4288,7 +4340,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4304,7 +4358,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4320,7 +4376,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -4429,7 +4487,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="15.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -4461,7 +4519,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4477,7 +4537,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4493,7 +4555,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -4605,7 +4669,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="13.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="8" max="16384" style="2" width="29.85546875" collapsed="true"/>
   </cols>
@@ -4639,7 +4703,9 @@
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>552</v>
+      </c>
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4658,7 +4724,9 @@
       <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="14" t="s">
+        <v>553</v>
+      </c>
       <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4677,7 +4745,9 @@
       <c r="E4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="14" t="s">
+        <v>553</v>
+      </c>
       <c r="G4" s="14"/>
     </row>
   </sheetData>
@@ -4701,7 +4771,7 @@
     <col min="2" max="3" bestFit="true" customWidth="true" style="2" width="32.0" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="28.140625" collapsed="true"/>
   </cols>
@@ -4735,7 +4805,9 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4754,7 +4826,9 @@
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4773,7 +4847,9 @@
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="G4" s="4"/>
     </row>
   </sheetData>
@@ -4896,7 +4972,7 @@
     <col min="4" max="4" customWidth="true" style="2" width="32.7109375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="9" max="9" style="2" width="9.140625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -4936,7 +5012,9 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4958,7 +5036,9 @@
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4980,7 +5060,9 @@
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="H4" s="4"/>
     </row>
   </sheetData>
@@ -5110,7 +5192,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="19.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="16384" style="2" width="53.5703125" collapsed="true"/>
   </cols>
@@ -5140,7 +5222,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5156,7 +5240,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5172,7 +5258,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -5282,7 +5370,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="22.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="16384" style="2" width="53.5703125" collapsed="true"/>
   </cols>
@@ -5312,7 +5400,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5328,7 +5418,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5344,7 +5436,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5360,7 +5454,9 @@
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F5" s="4"/>
     </row>
   </sheetData>
@@ -5485,7 +5581,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="13.5703125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="16384" style="2" width="53.5703125" collapsed="true"/>
   </cols>
@@ -5515,7 +5611,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5531,7 +5629,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5547,7 +5647,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5563,7 +5665,9 @@
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F5" s="4"/>
     </row>
   </sheetData>
@@ -5784,7 +5888,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="33.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="21.0" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="16384" style="2" width="53.5703125" collapsed="true"/>
   </cols>
@@ -5814,7 +5918,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5830,7 +5936,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5846,7 +5954,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -5955,7 +6065,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="16.85546875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -5987,7 +6097,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6003,7 +6115,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6019,7 +6133,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -6128,7 +6244,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="26.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="16.85546875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -6160,7 +6276,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6176,7 +6294,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6192,7 +6312,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -6301,7 +6423,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="36.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -6333,7 +6455,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6349,7 +6473,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6365,7 +6491,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -6474,7 +6602,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="13.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -6506,7 +6634,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6522,7 +6652,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6538,7 +6670,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -6649,7 +6783,7 @@
     <col min="2" max="3" bestFit="true" customWidth="true" style="2" width="39.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="13.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="7.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="8" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
@@ -6683,7 +6817,9 @@
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>552</v>
+      </c>
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6702,7 +6838,9 @@
       <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="14" t="s">
+        <v>553</v>
+      </c>
       <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6744,7 +6882,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="24.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -6776,7 +6914,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6792,7 +6932,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6808,7 +6950,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -6917,7 +7061,7 @@
     <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="23.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="24.0" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -6949,7 +7093,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6965,7 +7111,9 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6981,7 +7129,9 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
   </sheetData>
@@ -7091,7 +7241,7 @@
     <col min="2" max="2" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="26.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="7" max="7" style="2" width="9.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="28.140625" collapsed="true"/>
@@ -7123,7 +7273,9 @@
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>552</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8612,7 +8764,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="16.7109375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="9" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
@@ -8672,7 +8824,9 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8694,7 +8848,9 @@
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="H4" s="4"/>
     </row>
   </sheetData>
@@ -9562,7 +9718,7 @@
     <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="23.5703125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="10" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
@@ -9732,7 +9888,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="F3" s="14"/>
     </row>
@@ -9750,7 +9906,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="F4" s="14"/>
     </row>
@@ -9916,7 +10072,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="G3" s="14"/>
     </row>
@@ -9937,7 +10093,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="G4" s="14"/>
     </row>
@@ -10105,7 +10261,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="F3" s="14"/>
     </row>
@@ -10123,7 +10279,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="F4" s="14"/>
     </row>
@@ -10273,7 +10429,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="E3" s="4"/>
     </row>
@@ -10606,7 +10762,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="11.7109375" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="11" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
@@ -10652,7 +10808,9 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>552</v>
+      </c>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10680,7 +10838,9 @@
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10708,7 +10868,9 @@
       <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>553</v>
+      </c>
       <c r="J4" s="4"/>
     </row>
   </sheetData>
@@ -10864,7 +11026,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -10971,7 +11133,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>137</v>
+        <v>553</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -11953,7 +12115,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.58203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="5.85546875" collapsed="true"/>
     <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>

</xml_diff>